<commit_message>
working base + octaves
</commit_message>
<xml_diff>
--- a/resources/scales/Scales-Standard.xlsx
+++ b/resources/scales/Scales-Standard.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\creat\Desktop\Harmony-Engines-and-Scrapers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\creat\Desktop\Harmony-Engines-and-Scrapers\resources\scales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E46D82D0-FD9C-42DB-8163-47913750E7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F37AC35-D229-49A9-973F-4179F09AA4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{7F1C775B-60A2-4E31-B319-8D46D122CE06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{7F1C775B-60A2-4E31-B319-8D46D122CE06}"/>
   </bookViews>
   <sheets>
     <sheet name="Ecclesiastical Modes" sheetId="1" r:id="rId1"/>
-    <sheet name="Bebob, Blues and more" sheetId="2" r:id="rId2"/>
+    <sheet name="Bebop" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -849,7 +849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F095A36-20BE-4FE1-8B37-9ED53A3814E0}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -870,7 +870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -884,7 +884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -896,7 +896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -908,7 +908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>13</v>
@@ -920,7 +920,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -932,7 +932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>19</v>
@@ -944,7 +944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>22</v>
@@ -956,7 +956,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -970,7 +970,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
         <v>29</v>
@@ -982,7 +982,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="2" t="s">
         <v>32</v>
@@ -994,7 +994,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
         <v>35</v>
@@ -1006,7 +1006,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
         <v>38</v>
@@ -1018,7 +1018,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
         <v>41</v>
@@ -1030,7 +1030,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
         <v>44</v>
@@ -1042,7 +1042,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
         <v>51</v>
@@ -1068,7 +1068,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
         <v>54</v>
@@ -1080,7 +1080,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
         <v>57</v>
@@ -1092,7 +1092,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
         <v>60</v>
@@ -1104,7 +1104,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
         <v>63</v>
@@ -1116,7 +1116,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
         <v>66</v>
@@ -1142,7 +1142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B16C855-4FD8-4524-A5C5-D615386088DD}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1163,7 +1163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>69</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>73</v>
@@ -1201,7 +1201,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>77</v>
@@ -1213,7 +1213,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>79</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>82</v>
@@ -1239,7 +1239,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>84</v>
@@ -1251,7 +1251,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
         <v>87</v>
@@ -1263,7 +1263,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
         <v>90</v>
@@ -1275,7 +1275,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>92</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
         <v>96</v>
@@ -1301,7 +1301,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
         <v>99</v>
@@ -1313,7 +1313,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
         <v>101</v>
@@ -1325,7 +1325,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>103</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
         <v>107</v>
@@ -1351,7 +1351,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
         <v>110</v>
@@ -1363,7 +1363,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
         <v>112</v>
@@ -1375,7 +1375,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
         <v>89</v>
@@ -1387,7 +1387,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>114</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
         <v>114</v>
@@ -1413,7 +1413,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
         <v>120</v>
@@ -1425,7 +1425,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>122</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="2" t="s">
         <v>95</v>
@@ -1451,7 +1451,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
         <v>125</v>
@@ -1463,7 +1463,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="2" t="s">
         <v>127</v>
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="2" t="s">
         <v>130</v>
@@ -1487,7 +1487,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="2" t="s">
         <v>133</v>
@@ -1499,7 +1499,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="2" t="s">
         <v>98</v>
@@ -1511,7 +1511,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
         <v>135</v>
@@ -1547,7 +1547,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
         <v>141</v>
@@ -1559,7 +1559,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
         <v>144</v>
@@ -1571,7 +1571,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
         <v>146</v>
@@ -1585,12 +1585,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A23:A35"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>